<commit_message>
Remove useless thing in Job
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiril\Desktop\ConsoleScheduleCreator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\ConsoleScheduleCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2805" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7476" windowHeight="2808" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="4" r:id="rId1"/>
@@ -440,13 +440,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +454,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -462,7 +462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -470,7 +470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -478,7 +478,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -496,20 +496,20 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="5.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -532,7 +532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -555,7 +555,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -578,7 +578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -601,7 +601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -647,7 +647,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -670,7 +670,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -693,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -722,7 +722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -750,12 +750,12 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -769,7 +769,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -783,12 +783,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -802,7 +802,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -816,7 +816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3</v>
       </c>
@@ -830,7 +830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>4</v>
       </c>
@@ -844,7 +844,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>5</v>
       </c>
@@ -858,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>6</v>
       </c>
@@ -872,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -886,7 +886,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>

</xml_diff>